<commit_message>
Begun changes to integrate filter and analysis.
</commit_message>
<xml_diff>
--- a/outline.xlsx
+++ b/outline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="13050" windowHeight="8010"/>
+    <workbookView xWindow="2100" yWindow="105" windowWidth="13050" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Algo" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Ideas</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>can use to tell if hitting tilted syringe</t>
+  </si>
+  <si>
+    <t>Savefigures as svg pdfs….? (faster?)</t>
   </si>
 </sst>
 </file>
@@ -553,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,10 +850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,6 +918,11 @@
         <v>56</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>